<commit_message>
created ensembl id api script and finished custom scrublet for healthy
</commit_message>
<xml_diff>
--- a/sample_list_healthy.xlsx
+++ b/sample_list_healthy.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\randymi\Desktop\seuratwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B21A57-D923-4E01-80C0-301E27A08EDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FF1765-8384-4C51-8DBD-CE43D8667FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="samples" sheetId="1" r:id="rId1"/>
     <sheet name="key" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">samples!$A$1:$V$114</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -199,12 +202,37 @@
 Same as GSE249622 and 249793 but with different cell filtering. Shares supplement with GSE 249622</t>
       </text>
     </comment>
+    <comment ref="F109" authorId="3" shapeId="0" xr:uid="{235335E3-4B6D-4D5E-8985-A1F053CA83C3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>randymi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+good doublets
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="275">
   <si>
     <t>GSE</t>
   </si>
@@ -1026,6 +1054,9 @@
   </si>
   <si>
     <t>Lesional</t>
+  </si>
+  <si>
+    <t>sc</t>
   </si>
 </sst>
 </file>
@@ -1035,11 +1066,18 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1125,6 +1163,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="24">
@@ -1293,184 +1344,193 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1742,8 +1802,8 @@
   <dimension ref="A1:V1008"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E69" sqref="E69"/>
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1859,7 +1919,7 @@
       </c>
       <c r="J2" s="40"/>
       <c r="K2" s="25" t="b">
-        <f>NOT(O2)</f>
+        <f t="shared" ref="K2:K16" si="0">NOT(O2)</f>
         <v>0</v>
       </c>
       <c r="L2" s="32">
@@ -1888,7 +1948,7 @@
         <v>42.22</v>
       </c>
       <c r="U2" s="12">
-        <f t="shared" ref="U2:U10" si="0">14/5</f>
+        <f t="shared" ref="U2:U10" si="1">14/5</f>
         <v>2.8</v>
       </c>
       <c r="V2" s="5"/>
@@ -1917,7 +1977,7 @@
       </c>
       <c r="J3" s="40"/>
       <c r="K3" s="25" t="b">
-        <f>NOT(O3)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L3" s="32">
@@ -1946,7 +2006,7 @@
         <v>42.22</v>
       </c>
       <c r="U3" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.8</v>
       </c>
       <c r="V3" s="5"/>
@@ -1975,7 +2035,7 @@
       </c>
       <c r="J4" s="40"/>
       <c r="K4" s="25" t="b">
-        <f>NOT(O4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L4" s="32">
@@ -2004,7 +2064,7 @@
         <v>42.22</v>
       </c>
       <c r="U4" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.8</v>
       </c>
       <c r="V4" s="5"/>
@@ -2031,7 +2091,7 @@
       </c>
       <c r="J5" s="40"/>
       <c r="K5" s="25" t="b">
-        <f>NOT(O5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L5" s="32">
@@ -2060,7 +2120,7 @@
         <v>42.22</v>
       </c>
       <c r="U5" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.8</v>
       </c>
       <c r="V5" s="5"/>
@@ -2089,7 +2149,7 @@
       </c>
       <c r="J6" s="40"/>
       <c r="K6" s="25" t="b">
-        <f>NOT(O6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L6" s="32">
@@ -2118,7 +2178,7 @@
         <v>42.22</v>
       </c>
       <c r="U6" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.8</v>
       </c>
       <c r="V6" s="5"/>
@@ -2145,7 +2205,7 @@
       </c>
       <c r="J7" s="40"/>
       <c r="K7" s="25" t="b">
-        <f>NOT(O7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L7" s="32">
@@ -2174,7 +2234,7 @@
         <v>42.22</v>
       </c>
       <c r="U7" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.8</v>
       </c>
       <c r="V7" s="5"/>
@@ -2201,7 +2261,7 @@
       </c>
       <c r="J8" s="40"/>
       <c r="K8" s="25" t="b">
-        <f>NOT(O8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L8" s="32">
@@ -2230,7 +2290,7 @@
         <v>42.22</v>
       </c>
       <c r="U8" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.8</v>
       </c>
       <c r="V8" s="5"/>
@@ -2259,7 +2319,7 @@
       </c>
       <c r="J9" s="40"/>
       <c r="K9" s="25" t="b">
-        <f>NOT(O9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L9" s="32">
@@ -2288,7 +2348,7 @@
         <v>42.22</v>
       </c>
       <c r="U9" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.8</v>
       </c>
       <c r="V9" s="5"/>
@@ -2317,7 +2377,7 @@
       </c>
       <c r="J10" s="40"/>
       <c r="K10" s="25" t="b">
-        <f>NOT(O10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L10" s="32">
@@ -2346,7 +2406,7 @@
         <v>42.22</v>
       </c>
       <c r="U10" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.8</v>
       </c>
       <c r="V10" s="5"/>
@@ -2377,7 +2437,7 @@
       <c r="I11" s="43"/>
       <c r="J11" s="42"/>
       <c r="K11" s="25" t="b">
-        <f>NOT(O11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L11" s="37"/>
@@ -2408,13 +2468,19 @@
         <v>24</v>
       </c>
       <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
+      <c r="F12" s="43">
+        <v>2345</v>
+      </c>
+      <c r="G12" s="43">
+        <v>2205</v>
+      </c>
+      <c r="H12" s="82" t="s">
+        <v>23</v>
+      </c>
       <c r="I12" s="43"/>
       <c r="J12" s="43"/>
       <c r="K12" s="25" t="b">
-        <f>NOT(O12)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L12" s="25"/>
@@ -2445,13 +2511,19 @@
         <v>24</v>
       </c>
       <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
+      <c r="F13" s="43">
+        <v>1156</v>
+      </c>
+      <c r="G13" s="43">
+        <v>1015</v>
+      </c>
+      <c r="H13" s="82" t="s">
+        <v>23</v>
+      </c>
       <c r="I13" s="43"/>
       <c r="J13" s="43"/>
       <c r="K13" s="25" t="b">
-        <f>NOT(O13)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L13" s="25"/>
@@ -2482,13 +2554,19 @@
         <v>24</v>
       </c>
       <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
+      <c r="F14" s="43">
+        <v>1064</v>
+      </c>
+      <c r="G14" s="43">
+        <v>937</v>
+      </c>
+      <c r="H14" s="82" t="s">
+        <v>23</v>
+      </c>
       <c r="I14" s="43"/>
       <c r="J14" s="43"/>
       <c r="K14" s="25" t="b">
-        <f>NOT(O14)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L14" s="25"/>
@@ -2519,13 +2597,19 @@
         <v>24</v>
       </c>
       <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
+      <c r="F15" s="43">
+        <v>2438</v>
+      </c>
+      <c r="G15" s="43">
+        <v>2186</v>
+      </c>
+      <c r="H15" s="82" t="s">
+        <v>23</v>
+      </c>
       <c r="I15" s="43"/>
       <c r="J15" s="43"/>
       <c r="K15" s="25" t="b">
-        <f>NOT(O15)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L15" s="25"/>
@@ -2556,13 +2640,19 @@
         <v>24</v>
       </c>
       <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="43"/>
+      <c r="F16" s="82">
+        <v>2880</v>
+      </c>
+      <c r="G16" s="43">
+        <v>2754</v>
+      </c>
+      <c r="H16" s="82" t="s">
+        <v>23</v>
+      </c>
       <c r="I16" s="43"/>
       <c r="J16" s="43"/>
       <c r="K16" s="25" t="b">
-        <f>NOT(O16)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L16" s="25"/>
@@ -2633,13 +2723,19 @@
         <v>24</v>
       </c>
       <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
+      <c r="F18" s="82">
+        <v>2295</v>
+      </c>
+      <c r="G18" s="43">
+        <v>2210</v>
+      </c>
+      <c r="H18" s="82" t="s">
+        <v>23</v>
+      </c>
       <c r="I18" s="43"/>
       <c r="J18" s="43"/>
       <c r="K18" s="25" t="b">
-        <f>NOT(O18)</f>
+        <f t="shared" ref="K18:K38" si="2">NOT(O18)</f>
         <v>1</v>
       </c>
       <c r="L18" s="25"/>
@@ -2680,7 +2776,7 @@
         <v>25</v>
       </c>
       <c r="K19" s="25" t="b">
-        <f>NOT(O19)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L19" s="32">
@@ -2731,7 +2827,7 @@
         <v>25</v>
       </c>
       <c r="K20" s="25" t="b">
-        <f>NOT(O20)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L20" s="32">
@@ -2784,7 +2880,7 @@
         <v>30</v>
       </c>
       <c r="K21" s="25" t="b">
-        <f>NOT(O21)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L21" s="32">
@@ -2837,7 +2933,7 @@
         <v>30</v>
       </c>
       <c r="K22" s="25" t="b">
-        <f>NOT(O22)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L22" s="32">
@@ -2878,15 +2974,21 @@
         <v>24</v>
       </c>
       <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
+      <c r="F23" s="46">
+        <v>12952</v>
+      </c>
+      <c r="G23" s="46">
+        <v>11815</v>
+      </c>
+      <c r="H23" s="46" t="s">
+        <v>23</v>
+      </c>
       <c r="I23" s="46"/>
       <c r="J23" s="47" t="s">
         <v>25</v>
       </c>
       <c r="K23" s="25" t="b">
-        <f>NOT(O23)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L23" s="30"/>
@@ -2919,15 +3021,21 @@
         <v>24</v>
       </c>
       <c r="E24" s="46"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="46"/>
+      <c r="F24" s="46">
+        <v>11341</v>
+      </c>
+      <c r="G24" s="46">
+        <v>9955</v>
+      </c>
+      <c r="H24" s="46" t="s">
+        <v>23</v>
+      </c>
       <c r="I24" s="46"/>
       <c r="J24" s="47" t="s">
         <v>25</v>
       </c>
       <c r="K24" s="25" t="b">
-        <f>NOT(O24)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L24" s="30"/>
@@ -2960,17 +3068,23 @@
         <v>24</v>
       </c>
       <c r="E25" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="46"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="46"/>
+        <v>274</v>
+      </c>
+      <c r="F25" s="46">
+        <v>15777</v>
+      </c>
+      <c r="G25" s="46">
+        <v>7288</v>
+      </c>
+      <c r="H25" s="46" t="s">
+        <v>23</v>
+      </c>
       <c r="I25" s="46"/>
       <c r="J25" s="47" t="s">
         <v>30</v>
       </c>
       <c r="K25" s="25" t="b">
-        <f>NOT(O25)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L25" s="30"/>
@@ -3005,15 +3119,21 @@
       <c r="E26" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
+      <c r="F26" s="46">
+        <v>7223</v>
+      </c>
+      <c r="G26" s="46">
+        <v>6819</v>
+      </c>
+      <c r="H26" s="46" t="s">
+        <v>23</v>
+      </c>
       <c r="I26" s="46"/>
       <c r="J26" s="47" t="s">
         <v>30</v>
       </c>
       <c r="K26" s="25" t="b">
-        <f>NOT(O26)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L26" s="30"/>
@@ -3054,7 +3174,7 @@
       </c>
       <c r="J27" s="51"/>
       <c r="K27" s="25" t="b">
-        <f>NOT(O27)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L27" s="32">
@@ -3109,7 +3229,7 @@
       </c>
       <c r="J28" s="51"/>
       <c r="K28" s="25" t="b">
-        <f>NOT(O28)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L28" s="32">
@@ -3164,7 +3284,7 @@
       </c>
       <c r="J29" s="51"/>
       <c r="K29" s="25" t="b">
-        <f>NOT(O29)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L29" s="32">
@@ -3211,13 +3331,19 @@
         <v>24</v>
       </c>
       <c r="E30" s="53"/>
-      <c r="F30" s="53"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="53"/>
+      <c r="F30" s="53">
+        <v>9773</v>
+      </c>
+      <c r="G30" s="53">
+        <v>7356</v>
+      </c>
+      <c r="H30" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="I30" s="53"/>
       <c r="J30" s="54"/>
       <c r="K30" s="25" t="b">
-        <f>NOT(O30)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L30" s="30"/>
@@ -3266,7 +3392,7 @@
       </c>
       <c r="J31" s="57"/>
       <c r="K31" s="25" t="b">
-        <f>NOT(O31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L31" s="32">
@@ -3315,7 +3441,7 @@
       </c>
       <c r="J32" s="57"/>
       <c r="K32" s="25" t="b">
-        <f>NOT(O32)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L32" s="32">
@@ -3364,7 +3490,7 @@
       </c>
       <c r="J33" s="57"/>
       <c r="K33" s="25" t="b">
-        <f>NOT(O33)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L33" s="32">
@@ -3411,7 +3537,7 @@
       </c>
       <c r="J34" s="57"/>
       <c r="K34" s="25" t="b">
-        <f>NOT(O34)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L34" s="32">
@@ -3458,7 +3584,7 @@
       </c>
       <c r="J35" s="57"/>
       <c r="K35" s="25" t="b">
-        <f>NOT(O35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L35" s="32">
@@ -3507,7 +3633,7 @@
       </c>
       <c r="J36" s="57"/>
       <c r="K36" s="25" t="b">
-        <f>NOT(O36)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L36" s="32">
@@ -3556,7 +3682,7 @@
       </c>
       <c r="J37" s="57"/>
       <c r="K37" s="25" t="b">
-        <f>NOT(O37)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L37" s="32">
@@ -3605,7 +3731,7 @@
       </c>
       <c r="J38" s="57"/>
       <c r="K38" s="25" t="b">
-        <f>NOT(O38)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L38" s="32">
@@ -4400,13 +4526,19 @@
         <v>24</v>
       </c>
       <c r="E57" s="59"/>
-      <c r="F57" s="59"/>
-      <c r="G57" s="59"/>
-      <c r="H57" s="59"/>
+      <c r="F57" s="59">
+        <v>2582</v>
+      </c>
+      <c r="G57" s="59">
+        <v>2426</v>
+      </c>
+      <c r="H57" s="59" t="s">
+        <v>23</v>
+      </c>
       <c r="I57" s="59"/>
       <c r="J57" s="60"/>
       <c r="K57" s="25" t="b">
-        <f>NOT(O57)</f>
+        <f t="shared" ref="K57:K69" si="3">NOT(O57)</f>
         <v>1</v>
       </c>
       <c r="L57" s="30"/>
@@ -4443,13 +4575,19 @@
         <v>24</v>
       </c>
       <c r="E58" s="59"/>
-      <c r="F58" s="59"/>
-      <c r="G58" s="59"/>
-      <c r="H58" s="59"/>
+      <c r="F58" s="59">
+        <v>1033</v>
+      </c>
+      <c r="G58" s="59">
+        <v>859</v>
+      </c>
+      <c r="H58" s="59" t="s">
+        <v>23</v>
+      </c>
       <c r="I58" s="59"/>
       <c r="J58" s="60"/>
       <c r="K58" s="25" t="b">
-        <f>NOT(O58)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L58" s="30"/>
@@ -4496,7 +4634,7 @@
       <c r="I59" s="80"/>
       <c r="J59" s="81"/>
       <c r="K59" s="25" t="b">
-        <f>NOT(O59)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L59" s="30"/>
@@ -4533,13 +4671,19 @@
         <v>24</v>
       </c>
       <c r="E60" s="59"/>
-      <c r="F60" s="59"/>
-      <c r="G60" s="59"/>
-      <c r="H60" s="59"/>
+      <c r="F60" s="59">
+        <v>1531</v>
+      </c>
+      <c r="G60" s="59">
+        <v>1362</v>
+      </c>
+      <c r="H60" s="59" t="s">
+        <v>23</v>
+      </c>
       <c r="I60" s="59"/>
       <c r="J60" s="60"/>
       <c r="K60" s="25" t="b">
-        <f>NOT(O60)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L60" s="30"/>
@@ -4586,7 +4730,7 @@
       <c r="I61" s="80"/>
       <c r="J61" s="81"/>
       <c r="K61" s="25" t="b">
-        <f>NOT(O61)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L61" s="30"/>
@@ -4623,13 +4767,19 @@
         <v>24</v>
       </c>
       <c r="E62" s="59"/>
-      <c r="F62" s="59"/>
-      <c r="G62" s="59"/>
-      <c r="H62" s="59"/>
+      <c r="F62" s="59">
+        <v>1171</v>
+      </c>
+      <c r="G62" s="59">
+        <v>576</v>
+      </c>
+      <c r="H62" s="59" t="s">
+        <v>23</v>
+      </c>
       <c r="I62" s="59"/>
       <c r="J62" s="60"/>
       <c r="K62" s="25" t="b">
-        <f>NOT(O62)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L62" s="30"/>
@@ -4666,13 +4816,19 @@
         <v>24</v>
       </c>
       <c r="E63" s="59"/>
-      <c r="F63" s="59"/>
-      <c r="G63" s="59"/>
-      <c r="H63" s="59"/>
+      <c r="F63" s="59">
+        <v>839</v>
+      </c>
+      <c r="G63" s="59">
+        <v>561</v>
+      </c>
+      <c r="H63" s="59" t="s">
+        <v>23</v>
+      </c>
       <c r="I63" s="59"/>
       <c r="J63" s="60"/>
       <c r="K63" s="25" t="b">
-        <f>NOT(O63)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L63" s="30"/>
@@ -4709,13 +4865,19 @@
         <v>24</v>
       </c>
       <c r="E64" s="59"/>
-      <c r="F64" s="59"/>
-      <c r="G64" s="59"/>
-      <c r="H64" s="59"/>
+      <c r="F64" s="59">
+        <v>3871</v>
+      </c>
+      <c r="G64" s="59">
+        <v>2734</v>
+      </c>
+      <c r="H64" s="59" t="s">
+        <v>23</v>
+      </c>
       <c r="I64" s="59"/>
       <c r="J64" s="60"/>
       <c r="K64" s="25" t="b">
-        <f>NOT(O64)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L64" s="30"/>
@@ -4752,13 +4914,19 @@
         <v>24</v>
       </c>
       <c r="E65" s="59"/>
-      <c r="F65" s="59"/>
-      <c r="G65" s="59"/>
-      <c r="H65" s="59"/>
+      <c r="F65" s="59">
+        <v>2615</v>
+      </c>
+      <c r="G65" s="59">
+        <v>2263</v>
+      </c>
+      <c r="H65" s="59" t="s">
+        <v>23</v>
+      </c>
       <c r="I65" s="59"/>
       <c r="J65" s="60"/>
       <c r="K65" s="25" t="b">
-        <f>NOT(O65)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L65" s="30"/>
@@ -4795,13 +4963,19 @@
         <v>24</v>
       </c>
       <c r="E66" s="59"/>
-      <c r="F66" s="59"/>
-      <c r="G66" s="59"/>
-      <c r="H66" s="59"/>
+      <c r="F66" s="59">
+        <v>2490</v>
+      </c>
+      <c r="G66" s="59">
+        <v>1485</v>
+      </c>
+      <c r="H66" s="59" t="s">
+        <v>23</v>
+      </c>
       <c r="I66" s="59"/>
       <c r="J66" s="60"/>
       <c r="K66" s="25" t="b">
-        <f>NOT(O66)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L66" s="30"/>
@@ -4846,7 +5020,7 @@
       <c r="I67" s="5"/>
       <c r="J67" s="26"/>
       <c r="K67" s="25" t="b">
-        <f>NOT(O67)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L67" s="30"/>
@@ -4887,7 +5061,7 @@
       <c r="I68" s="5"/>
       <c r="J68" s="26"/>
       <c r="K68" s="25" t="b">
-        <f>NOT(O68)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L68" s="30"/>
@@ -4928,7 +5102,7 @@
       <c r="I69" s="5"/>
       <c r="J69" s="26"/>
       <c r="K69" s="25" t="b">
-        <f>NOT(O69)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L69" s="30"/>
@@ -5011,7 +5185,7 @@
         <v>30</v>
       </c>
       <c r="K71" s="25" t="b">
-        <f>NOT(O71)</f>
+        <f t="shared" ref="K71:K114" si="4">NOT(O71)</f>
         <v>0</v>
       </c>
       <c r="L71" s="32">
@@ -5066,7 +5240,7 @@
         <v>30</v>
       </c>
       <c r="K72" s="25" t="b">
-        <f>NOT(O72)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L72" s="32">
@@ -5121,7 +5295,7 @@
         <v>30</v>
       </c>
       <c r="K73" s="25" t="b">
-        <f>NOT(O73)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L73" s="32">
@@ -5166,15 +5340,19 @@
         <v>24</v>
       </c>
       <c r="E74" s="62"/>
-      <c r="F74" s="62"/>
-      <c r="G74" s="62"/>
+      <c r="F74" s="62">
+        <v>3930</v>
+      </c>
+      <c r="G74" s="62">
+        <v>2623</v>
+      </c>
       <c r="H74" s="62"/>
       <c r="I74" s="62"/>
       <c r="J74" s="63" t="s">
         <v>30</v>
       </c>
       <c r="K74" s="25" t="b">
-        <f>NOT(O74)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L74" s="30"/>
@@ -5207,15 +5385,19 @@
         <v>24</v>
       </c>
       <c r="E75" s="62"/>
-      <c r="F75" s="62"/>
-      <c r="G75" s="62"/>
+      <c r="F75" s="62">
+        <v>5474</v>
+      </c>
+      <c r="G75" s="62">
+        <v>5163</v>
+      </c>
       <c r="H75" s="62"/>
       <c r="I75" s="62"/>
       <c r="J75" s="63" t="s">
         <v>30</v>
       </c>
       <c r="K75" s="25" t="b">
-        <f>NOT(O75)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L75" s="30"/>
@@ -5248,15 +5430,19 @@
         <v>24</v>
       </c>
       <c r="E76" s="62"/>
-      <c r="F76" s="62"/>
-      <c r="G76" s="62"/>
+      <c r="F76" s="62">
+        <v>5972</v>
+      </c>
+      <c r="G76" s="62">
+        <v>5692</v>
+      </c>
       <c r="H76" s="62"/>
       <c r="I76" s="62"/>
       <c r="J76" s="63" t="s">
         <v>30</v>
       </c>
       <c r="K76" s="25" t="b">
-        <f>NOT(O76)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L76" s="30"/>
@@ -5289,15 +5475,19 @@
         <v>24</v>
       </c>
       <c r="E77" s="62"/>
-      <c r="F77" s="62"/>
-      <c r="G77" s="62"/>
+      <c r="F77" s="62">
+        <v>1806</v>
+      </c>
+      <c r="G77" s="62">
+        <v>1749</v>
+      </c>
       <c r="H77" s="62"/>
       <c r="I77" s="62"/>
       <c r="J77" s="63" t="s">
         <v>30</v>
       </c>
       <c r="K77" s="25" t="b">
-        <f>NOT(O77)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L77" s="30"/>
@@ -5330,15 +5520,19 @@
         <v>24</v>
       </c>
       <c r="E78" s="62"/>
-      <c r="F78" s="62"/>
-      <c r="G78" s="62"/>
+      <c r="F78" s="62">
+        <v>4909</v>
+      </c>
+      <c r="G78" s="62">
+        <v>3984</v>
+      </c>
       <c r="H78" s="62"/>
       <c r="I78" s="62"/>
       <c r="J78" s="63" t="s">
         <v>30</v>
       </c>
       <c r="K78" s="25" t="b">
-        <f>NOT(O78)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L78" s="30"/>
@@ -5371,15 +5565,19 @@
         <v>24</v>
       </c>
       <c r="E79" s="62"/>
-      <c r="F79" s="62"/>
-      <c r="G79" s="62"/>
+      <c r="F79" s="62">
+        <v>6180</v>
+      </c>
+      <c r="G79" s="62">
+        <v>5907</v>
+      </c>
       <c r="H79" s="62"/>
       <c r="I79" s="62"/>
       <c r="J79" s="63" t="s">
         <v>30</v>
       </c>
       <c r="K79" s="25" t="b">
-        <f>NOT(O79)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L79" s="30"/>
@@ -5422,7 +5620,7 @@
         <v>95</v>
       </c>
       <c r="K80" s="25" t="b">
-        <f>NOT(O80)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L80" s="32">
@@ -5471,7 +5669,7 @@
         <v>98</v>
       </c>
       <c r="K81" s="25" t="b">
-        <f>NOT(O81)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L81" s="32">
@@ -5526,7 +5724,7 @@
         <v>100</v>
       </c>
       <c r="K82" s="25" t="b">
-        <f>NOT(O82)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L82" s="32">
@@ -5581,7 +5779,7 @@
         <v>100</v>
       </c>
       <c r="K83" s="25" t="b">
-        <f>NOT(O83)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L83" s="32">
@@ -5636,7 +5834,7 @@
         <v>98</v>
       </c>
       <c r="K84" s="25" t="b">
-        <f>NOT(O84)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L84" s="32">
@@ -5691,7 +5889,7 @@
         <v>98</v>
       </c>
       <c r="K85" s="25" t="b">
-        <f>NOT(O85)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L85" s="32">
@@ -5746,7 +5944,7 @@
         <v>100</v>
       </c>
       <c r="K86" s="25" t="b">
-        <f>NOT(O86)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L86" s="32">
@@ -5801,7 +5999,7 @@
         <v>95</v>
       </c>
       <c r="K87" s="25" t="b">
-        <f>NOT(O87)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L87" s="32">
@@ -5833,28 +6031,30 @@
       <c r="V87" s="5"/>
     </row>
     <row r="88" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A88" s="70" t="s">
+      <c r="A88" s="83" t="s">
         <v>93</v>
       </c>
-      <c r="B88" s="71" t="s">
+      <c r="B88" s="84" t="s">
         <v>105</v>
       </c>
-      <c r="C88" s="71" t="s">
-        <v>23</v>
-      </c>
-      <c r="D88" s="71" t="s">
+      <c r="C88" s="84" t="s">
+        <v>23</v>
+      </c>
+      <c r="D88" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="E88" s="71"/>
-      <c r="F88" s="71"/>
-      <c r="G88" s="71"/>
-      <c r="H88" s="71"/>
-      <c r="I88" s="71"/>
+      <c r="E88" s="84"/>
+      <c r="F88" s="84">
+        <v>457</v>
+      </c>
+      <c r="G88" s="84"/>
+      <c r="H88" s="84"/>
+      <c r="I88" s="84"/>
       <c r="J88" s="72" t="s">
         <v>95</v>
       </c>
       <c r="K88" s="25" t="b">
-        <f>NOT(O88)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L88" s="30"/>
@@ -5887,15 +6087,21 @@
         <v>24</v>
       </c>
       <c r="E89" s="71"/>
-      <c r="F89" s="71"/>
-      <c r="G89" s="71"/>
-      <c r="H89" s="71"/>
+      <c r="F89" s="71">
+        <v>3518</v>
+      </c>
+      <c r="G89" s="71">
+        <v>3438</v>
+      </c>
+      <c r="H89" s="71" t="s">
+        <v>23</v>
+      </c>
       <c r="I89" s="71"/>
       <c r="J89" s="72" t="s">
         <v>95</v>
       </c>
       <c r="K89" s="25" t="b">
-        <f>NOT(O89)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L89" s="30"/>
@@ -5928,15 +6134,21 @@
         <v>24</v>
       </c>
       <c r="E90" s="71"/>
-      <c r="F90" s="71"/>
-      <c r="G90" s="71"/>
-      <c r="H90" s="71"/>
+      <c r="F90" s="71">
+        <v>2309</v>
+      </c>
+      <c r="G90" s="71">
+        <v>2225</v>
+      </c>
+      <c r="H90" s="71" t="s">
+        <v>23</v>
+      </c>
       <c r="I90" s="71"/>
       <c r="J90" s="72" t="s">
         <v>100</v>
       </c>
       <c r="K90" s="25" t="b">
-        <f>NOT(O90)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L90" s="30"/>
@@ -5969,15 +6181,21 @@
         <v>24</v>
       </c>
       <c r="E91" s="71"/>
-      <c r="F91" s="71"/>
-      <c r="G91" s="71"/>
-      <c r="H91" s="71"/>
+      <c r="F91" s="71">
+        <v>8907</v>
+      </c>
+      <c r="G91" s="71">
+        <v>8717</v>
+      </c>
+      <c r="H91" s="71" t="s">
+        <v>23</v>
+      </c>
       <c r="I91" s="71"/>
       <c r="J91" s="72" t="s">
         <v>98</v>
       </c>
       <c r="K91" s="25" t="b">
-        <f>NOT(O91)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L91" s="30"/>
@@ -6010,15 +6228,21 @@
         <v>24</v>
       </c>
       <c r="E92" s="71"/>
-      <c r="F92" s="71"/>
-      <c r="G92" s="71"/>
-      <c r="H92" s="71"/>
+      <c r="F92" s="71">
+        <v>8516</v>
+      </c>
+      <c r="G92" s="71">
+        <v>8359</v>
+      </c>
+      <c r="H92" s="71" t="s">
+        <v>23</v>
+      </c>
       <c r="I92" s="71"/>
       <c r="J92" s="72" t="s">
         <v>95</v>
       </c>
       <c r="K92" s="25" t="b">
-        <f>NOT(O92)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L92" s="30"/>
@@ -6051,15 +6275,21 @@
         <v>24</v>
       </c>
       <c r="E93" s="71"/>
-      <c r="F93" s="71"/>
-      <c r="G93" s="71"/>
-      <c r="H93" s="71"/>
+      <c r="F93" s="71">
+        <v>11346</v>
+      </c>
+      <c r="G93" s="71">
+        <v>11156</v>
+      </c>
+      <c r="H93" s="71" t="s">
+        <v>23</v>
+      </c>
       <c r="I93" s="71"/>
       <c r="J93" s="72" t="s">
         <v>95</v>
       </c>
       <c r="K93" s="25" t="b">
-        <f>NOT(O93)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L93" s="30"/>
@@ -6102,7 +6332,7 @@
         <v>113</v>
       </c>
       <c r="K94" s="25" t="b">
-        <f>NOT(O94)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L94" s="31">
@@ -6157,7 +6387,7 @@
         <v>113</v>
       </c>
       <c r="K95" s="25" t="b">
-        <f>NOT(O95)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L95" s="31">
@@ -6212,7 +6442,7 @@
         <v>113</v>
       </c>
       <c r="K96" s="25" t="b">
-        <f>NOT(O96)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L96" s="31">
@@ -6267,7 +6497,7 @@
         <v>113</v>
       </c>
       <c r="K97" s="25" t="b">
-        <f>NOT(O97)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L97" s="31">
@@ -6322,7 +6552,7 @@
         <v>113</v>
       </c>
       <c r="K98" s="25" t="b">
-        <f>NOT(O98)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L98" s="31">
@@ -6377,7 +6607,7 @@
         <v>113</v>
       </c>
       <c r="K99" s="25" t="b">
-        <f>NOT(O99)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L99" s="31">
@@ -6432,7 +6662,7 @@
         <v>113</v>
       </c>
       <c r="K100" s="25" t="b">
-        <f>NOT(O100)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L100" s="31">
@@ -6487,7 +6717,7 @@
         <v>113</v>
       </c>
       <c r="K101" s="25" t="b">
-        <f>NOT(O101)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L101" s="32">
@@ -6542,7 +6772,7 @@
         <v>113</v>
       </c>
       <c r="K102" s="25" t="b">
-        <f>NOT(O102)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L102" s="32">
@@ -6597,7 +6827,7 @@
         <v>113</v>
       </c>
       <c r="K103" s="25" t="b">
-        <f>NOT(O103)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L103" s="32">
@@ -6642,15 +6872,21 @@
         <v>24</v>
       </c>
       <c r="E104" s="74"/>
-      <c r="F104" s="74"/>
-      <c r="G104" s="74"/>
-      <c r="H104" s="74"/>
+      <c r="F104" s="74">
+        <v>4022</v>
+      </c>
+      <c r="G104" s="74">
+        <v>3701</v>
+      </c>
+      <c r="H104" s="74" t="s">
+        <v>23</v>
+      </c>
       <c r="I104" s="74"/>
       <c r="J104" s="75" t="s">
         <v>113</v>
       </c>
       <c r="K104" s="25" t="b">
-        <f>NOT(O104)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L104" s="30"/>
@@ -6670,20 +6906,22 @@
       <c r="V104" s="5"/>
     </row>
     <row r="105" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A105" s="73" t="s">
+      <c r="A105" s="85" t="s">
         <v>111</v>
       </c>
-      <c r="B105" s="74" t="s">
+      <c r="B105" s="86" t="s">
         <v>124</v>
       </c>
-      <c r="C105" s="74" t="s">
-        <v>23</v>
-      </c>
-      <c r="D105" s="74" t="s">
+      <c r="C105" s="86" t="s">
+        <v>23</v>
+      </c>
+      <c r="D105" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="E105" s="74"/>
-      <c r="F105" s="74"/>
+      <c r="E105" s="86"/>
+      <c r="F105" s="86">
+        <v>483</v>
+      </c>
       <c r="G105" s="74"/>
       <c r="H105" s="74"/>
       <c r="I105" s="74"/>
@@ -6691,7 +6929,7 @@
         <v>113</v>
       </c>
       <c r="K105" s="25" t="b">
-        <f>NOT(O105)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L105" s="30"/>
@@ -6724,15 +6962,21 @@
         <v>24</v>
       </c>
       <c r="E106" s="74"/>
-      <c r="F106" s="74"/>
-      <c r="G106" s="74"/>
-      <c r="H106" s="74"/>
+      <c r="F106" s="74">
+        <v>5604</v>
+      </c>
+      <c r="G106" s="74">
+        <v>5147</v>
+      </c>
+      <c r="H106" s="74" t="s">
+        <v>23</v>
+      </c>
       <c r="I106" s="74"/>
       <c r="J106" s="75" t="s">
         <v>113</v>
       </c>
       <c r="K106" s="25" t="b">
-        <f>NOT(O106)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L106" s="30"/>
@@ -6765,15 +7009,21 @@
         <v>24</v>
       </c>
       <c r="E107" s="74"/>
-      <c r="F107" s="74"/>
-      <c r="G107" s="74"/>
-      <c r="H107" s="74"/>
+      <c r="F107" s="74">
+        <v>4669</v>
+      </c>
+      <c r="G107" s="74">
+        <v>4460</v>
+      </c>
+      <c r="H107" s="74" t="s">
+        <v>23</v>
+      </c>
       <c r="I107" s="74"/>
       <c r="J107" s="75" t="s">
         <v>113</v>
       </c>
       <c r="K107" s="25" t="b">
-        <f>NOT(O107)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L107" s="30"/>
@@ -6806,15 +7056,21 @@
         <v>24</v>
       </c>
       <c r="E108" s="74"/>
-      <c r="F108" s="74"/>
-      <c r="G108" s="74"/>
-      <c r="H108" s="74"/>
+      <c r="F108" s="74">
+        <v>4970</v>
+      </c>
+      <c r="G108" s="74">
+        <v>4732</v>
+      </c>
+      <c r="H108" s="74" t="s">
+        <v>23</v>
+      </c>
       <c r="I108" s="74"/>
       <c r="J108" s="75" t="s">
         <v>113</v>
       </c>
       <c r="K108" s="25" t="b">
-        <f>NOT(O108)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L108" s="30"/>
@@ -6847,15 +7103,21 @@
         <v>24</v>
       </c>
       <c r="E109" s="74"/>
-      <c r="F109" s="74"/>
-      <c r="G109" s="74"/>
-      <c r="H109" s="74"/>
+      <c r="F109" s="74">
+        <v>9326</v>
+      </c>
+      <c r="G109" s="74">
+        <v>8774</v>
+      </c>
+      <c r="H109" s="74" t="s">
+        <v>23</v>
+      </c>
       <c r="I109" s="74"/>
       <c r="J109" s="75" t="s">
         <v>113</v>
       </c>
       <c r="K109" s="25" t="b">
-        <f>NOT(O109)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L109" s="30"/>
@@ -6875,20 +7137,22 @@
       <c r="V109" s="5"/>
     </row>
     <row r="110" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A110" s="73" t="s">
+      <c r="A110" s="85" t="s">
         <v>111</v>
       </c>
-      <c r="B110" s="74" t="s">
+      <c r="B110" s="86" t="s">
         <v>129</v>
       </c>
-      <c r="C110" s="74" t="s">
-        <v>23</v>
-      </c>
-      <c r="D110" s="74" t="s">
+      <c r="C110" s="86" t="s">
+        <v>23</v>
+      </c>
+      <c r="D110" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="E110" s="74"/>
-      <c r="F110" s="74"/>
+      <c r="E110" s="86"/>
+      <c r="F110" s="86">
+        <v>417</v>
+      </c>
       <c r="G110" s="74"/>
       <c r="H110" s="74"/>
       <c r="I110" s="74"/>
@@ -6896,7 +7160,7 @@
         <v>113</v>
       </c>
       <c r="K110" s="25" t="b">
-        <f>NOT(O110)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L110" s="30"/>
@@ -6929,15 +7193,21 @@
         <v>24</v>
       </c>
       <c r="E111" s="74"/>
-      <c r="F111" s="74"/>
-      <c r="G111" s="74"/>
-      <c r="H111" s="74"/>
+      <c r="F111" s="74">
+        <v>3897</v>
+      </c>
+      <c r="G111" s="74">
+        <v>3812</v>
+      </c>
+      <c r="H111" s="74" t="s">
+        <v>23</v>
+      </c>
       <c r="I111" s="74"/>
       <c r="J111" s="75" t="s">
         <v>113</v>
       </c>
       <c r="K111" s="25" t="b">
-        <f>NOT(O111)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L111" s="30"/>
@@ -6970,15 +7240,21 @@
         <v>24</v>
       </c>
       <c r="E112" s="74"/>
-      <c r="F112" s="74"/>
-      <c r="G112" s="74"/>
-      <c r="H112" s="74"/>
+      <c r="F112" s="74">
+        <v>6490</v>
+      </c>
+      <c r="G112" s="74">
+        <v>6349</v>
+      </c>
+      <c r="H112" s="74" t="s">
+        <v>23</v>
+      </c>
       <c r="I112" s="74"/>
       <c r="J112" s="75" t="s">
         <v>113</v>
       </c>
       <c r="K112" s="25" t="b">
-        <f>NOT(O112)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L112" s="30"/>
@@ -7011,15 +7287,21 @@
         <v>24</v>
       </c>
       <c r="E113" s="74"/>
-      <c r="F113" s="74"/>
-      <c r="G113" s="74"/>
-      <c r="H113" s="74"/>
+      <c r="F113" s="74">
+        <v>10847</v>
+      </c>
+      <c r="G113" s="74">
+        <v>10697</v>
+      </c>
+      <c r="H113" s="74" t="s">
+        <v>23</v>
+      </c>
       <c r="I113" s="74"/>
       <c r="J113" s="75" t="s">
         <v>113</v>
       </c>
       <c r="K113" s="25" t="b">
-        <f>NOT(O113)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L113" s="30"/>
@@ -7058,7 +7340,7 @@
       <c r="I114" s="34"/>
       <c r="J114" s="35"/>
       <c r="K114" s="25" t="b">
-        <f>NOT(O114)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L114" s="32">
@@ -7979,6 +8261,7 @@
     <row r="1007" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="1008" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
+  <autoFilter ref="A1:V114" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V1008">
     <sortCondition ref="A1:A1008"/>
   </sortState>
@@ -8179,7 +8462,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A9:A16">
     <cfRule type="colorScale" priority="1">
       <colorScale>

</xml_diff>